<commit_message>
added interface to get all companies, updated to dos, change password
</commit_message>
<xml_diff>
--- a/docs/ToDo Liste.xlsx
+++ b/docs/ToDo Liste.xlsx
@@ -20,12 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
   <si>
     <t xml:space="preserve">TEAM 8 TODO TABLE</t>
   </si>
   <si>
-    <t xml:space="preserve">VERSION 1.0.0</t>
+    <t xml:space="preserve">VERSION 3.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmierung Backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmierung Frontend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation/Sonstiges</t>
   </si>
   <si>
     <t xml:space="preserve">Dokumente</t>
@@ -40,184 +49,160 @@
     <t xml:space="preserve">TO DO</t>
   </si>
   <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bemerkung</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stand</t>
   </si>
   <si>
-    <t xml:space="preserve">Bemerkung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trello</t>
   </si>
   <si>
+    <t xml:space="preserve">Prototyp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erledigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bildung von Team Frontend und Team  Backend.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dies soll schleunigst getan werden. Spätestens am MONTAG! (Suada)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sequenzdiagramm</t>
   </si>
   <si>
+    <t xml:space="preserve">Pensum implementieren und Jobinserat dadurch erweitern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branche implementieren und damit Jobinserate erweitern  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technologien Kennenlernen</t>
+  </si>
+  <si>
     <t xml:space="preserve">UML Diagramm</t>
   </si>
   <si>
-    <t xml:space="preserve">Erledigt</t>
+    <t xml:space="preserve">Kontakt implementieren und Jobinserat dadruch erweitern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellung von weiteren Components (z.B-joblisting, newjoblisting, joblistingdetail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRUD Operationen für Jobinserate</t>
   </si>
   <si>
     <t xml:space="preserve">Requirements Specifications</t>
   </si>
   <si>
+    <t xml:space="preserve">Git Tafel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. - 14.Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentifizierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbindung der Components mittels Routing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deployment to Heroku</t>
+  </si>
+  <si>
     <t xml:space="preserve">Use Case Diagramm</t>
   </si>
   <si>
+    <t xml:space="preserve">Git Textdoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization vervollständigen; USER, INSERATE, SKILL. COMPANY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKILL wurde weggelassen (Simone)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation zwischen Subseiten verbessern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRUD Operationen für Benutzeradmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update und Delete sind noch nicht implementiert (Simone)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Designvorschlag</t>
   </si>
   <si>
     <t xml:space="preserve">Muss evtl. nach Manuels Wünschen überarbeitet werden. (Suada)</t>
   </si>
   <si>
-    <t xml:space="preserve">--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designvorschlag2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dieser ist für uns. Soll detaillierter sein. Darüber könnten wir am Montag 12.November reden.(Suada)</t>
+    <t xml:space="preserve">7- 14.Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin/ Moderator: Verifizierte User: Schnittstelle für isVerified-Flag Admin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporär: Bestätigen in Übersicht. (Timo (aus Textdoc)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellung einer Login Maske</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRUD Operationen für Inserate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update und Delete sind noch offen (Simone)</t>
   </si>
   <si>
     <t xml:space="preserve">Krähenfussdiagramm</t>
   </si>
   <si>
+    <t xml:space="preserve">7 - 14.Nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin/ Moderator: Verifizierte Inserate: Schnittstelle für isVerified-Flag Admin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04. - 12.Nov </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auflistung von Jobinseraten mit Detailansicht. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wir spätestens bis  Montag erledigt. (Suada)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usability Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabenblatt erstellen, Gedanken machen zu ‚How to...‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ablauf, ScreenCapture Tool?, laut denken &amp; notieren etc. (Simone)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fortlaufend</t>
   </si>
   <si>
     <t xml:space="preserve">Time Table wöchentlich ausfüllen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programmierung Backend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programmierung Frontend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation/Sonstiges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prototyp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bildung von Team Frontend und Team  Backend.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dies soll schleunigst getan werden. Spätestens am MONTAG! (Suada)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pensum implementieren und Jobinserat dadurch erweitern.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branche implementieren und damit Jobinserate erweitern  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milestone1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technologien Kennenlernen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kontakt implementieren und Jobinserat dadruch erweitern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erstellung von weiteren Components (z.B-joblisting, newjoblisting, joblistingdetail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRUD Operationen für Jobinserate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Git Tafel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. - 14.Nov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authentifizierung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbindung der Components mittels Routing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deployment to Heroku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Git Textdoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authorization vervollständigen; USER, INSERATE, SKILL. COMPANY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKILL wurde weggelassen (Simone)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigation zwischen Subseiten verbessern.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milestone2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRUD Operationen für Benutzeradmin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noch offen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update und Delete sind noch nicht implementiert (Simone)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7- 14.Nov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin/ Moderator: Verifizierte User: Schnittstelle für isVerified-Flag Admin.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temporär: Bestätigen in Übersicht. (Timo (aus Textdoc)) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erstellung einer Login Maske</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milestone 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRUD Operationen für Inserate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">update und Delete sind noch offen (Simone)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 - 14.Nov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin/ Moderator: Verifizierte Inserate: Schnittstelle für isVerified-Flag Admin.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04. - 12.Nov </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auflistung von Jobinseraten mit Detailansicht. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wir spätestens bis  Montag erledigt. (Suada)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usability Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufgabenblatt erstellen, Gedanken machen zu ‚How to...‘</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ablauf, ScreenCapture Tool?, laut denken &amp; notieren etc. (Simone)</t>
   </si>
   <si>
     <t xml:space="preserve">7. - 14.Nov</t>
@@ -241,6 +226,18 @@
     <t xml:space="preserve">Timo &amp; Michael (Simone)</t>
   </si>
   <si>
+    <t xml:space="preserve">Meeting 05.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designvorschlag2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dieser ist für uns. Soll detaillierter sein. Darüber könnten wir am Montag 12.November reden.(Suada)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filtermöglichkeiten (Backend)</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
     <t xml:space="preserve">Suchfunktion auf Jobinserate</t>
   </si>
   <si>
+    <t xml:space="preserve">Krähenfussdiagramm 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Meeting 21.11.</t>
   </si>
   <si>
@@ -268,6 +268,9 @@
     <t xml:space="preserve">Filterfunktion auf Jobinserate</t>
   </si>
   <si>
+    <t xml:space="preserve">Requirements Specifications überarbeiten</t>
+  </si>
+  <si>
     <t xml:space="preserve">DB erweitern mit Company.Website, Joblisting.Bewerbungsfrist</t>
   </si>
   <si>
@@ -277,7 +280,7 @@
     <t xml:space="preserve">Daten (z.B. companyId aus Token nehmen) (Simone)</t>
   </si>
   <si>
-    <t xml:space="preserve">Surprise feature</t>
+    <t xml:space="preserve">Surprise feature/ Bewerbungsbriefvorlage</t>
   </si>
   <si>
     <t xml:space="preserve">Needs to be cool and heapful for the </t>
@@ -314,16 +317,28 @@
     <t xml:space="preserve">Test auswerten</t>
   </si>
   <si>
+    <t xml:space="preserve">All Companies</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filtermöglichkeiten (Frontend)</t>
   </si>
   <si>
+    <t xml:space="preserve">Aufräumen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Registrieren: Deutsche Formulierung</t>
   </si>
   <si>
+    <t xml:space="preserve">Kommentieren</t>
+  </si>
+  <si>
     <t xml:space="preserve">wenn zu viel Zeit</t>
   </si>
   <si>
-    <t xml:space="preserve">CompanyId wird automatisch in Registering-Form eingefüllt</t>
+    <t xml:space="preserve">Company wird automatisch in Registering-Form eingefüllt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests</t>
   </si>
   <si>
     <t xml:space="preserve">für Admin: wenn Inserat/Benutzer zurückgewiesen wird, muss ein Kommentar erfasst werden können.</t>
@@ -359,7 +374,7 @@
     <numFmt numFmtId="165" formatCode="DD/\ MMM"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -398,6 +413,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -415,9 +437,8 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -569,7 +590,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,7 +623,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,15 +635,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -630,15 +647,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,11 +667,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -662,23 +683,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,7 +711,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -784,8 +809,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8165160" y="660600"/>
-          <a:ext cx="7077960" cy="3677040"/>
+          <a:off x="8051040" y="660600"/>
+          <a:ext cx="6972840" cy="3616200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1171,7 +1196,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>179640</xdr:colOff>
+      <xdr:colOff>180000</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>9000</xdr:rowOff>
     </xdr:from>
@@ -1179,7 +1204,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>678600</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>221400</xdr:rowOff>
+      <xdr:rowOff>221040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1193,8 +1218,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15333840" y="669960"/>
-          <a:ext cx="2099160" cy="3075480"/>
+          <a:off x="15114960" y="669960"/>
+          <a:ext cx="2079720" cy="3014280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1214,33 +1239,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:41"/>
+  <dimension ref="1:44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.25"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="41.0102040816327"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="18.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,14 +2329,12 @@
       <c r="Q3" s="0"/>
       <c r="R3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
       <c r="G4" s="6"/>
       <c r="H4" s="2"/>
       <c r="I4" s="0"/>
@@ -2318,22 +2347,12 @@
       <c r="Q4" s="0"/>
       <c r="R4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>7</v>
-      </c>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
       <c r="G5" s="6"/>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
@@ -2346,16 +2365,12 @@
       <c r="Q5" s="0"/>
       <c r="R5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
       <c r="G6" s="6"/>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
@@ -2368,20 +2383,12 @@
       <c r="Q6" s="0"/>
       <c r="R6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="15" t="n">
-        <v>43383</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="14"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
       <c r="G7" s="6"/>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
@@ -2395,19 +2402,11 @@
       <c r="R7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="15" t="n">
-        <v>43383</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="14"/>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
       <c r="G8" s="6"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
@@ -2421,19 +2420,11 @@
       <c r="R8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="15" t="n">
-        <v>43390</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="14"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
       <c r="G9" s="6"/>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
@@ -2447,21 +2438,11 @@
       <c r="R9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="15" t="n">
-        <v>43392</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
       <c r="G10" s="6"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
@@ -2475,19 +2456,11 @@
       <c r="R10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
       <c r="G11" s="6"/>
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
@@ -2501,19 +2474,11 @@
       <c r="R11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="15" t="n">
-        <v>43390</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="14"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
       <c r="G12" s="6"/>
       <c r="H12" s="0"/>
       <c r="I12" s="0"/>
@@ -2527,17 +2492,11 @@
       <c r="R12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="14"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
       <c r="G13" s="6"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
@@ -2551,7 +2510,7 @@
       <c r="R13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="16"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
@@ -2568,784 +2527,1013 @@
       <c r="Q14" s="0"/>
       <c r="R14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8" t="s">
-        <v>23</v>
+    <row r="15" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="8" t="s">
-        <v>24</v>
+      <c r="H15" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
-      <c r="N15" s="8" t="s">
-        <v>25</v>
+      <c r="N15" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="T15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>7</v>
       </c>
+      <c r="D16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="12" t="s">
+      <c r="H16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="12" t="s">
+      <c r="J16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="13" t="s">
         <v>7</v>
       </c>
+      <c r="P16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="U16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="X16" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="47.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="13" t="s">
-        <v>8</v>
+      <c r="B17" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>43381</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="12"/>
+      <c r="D17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="13"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="13" t="s">
-        <v>8</v>
+      <c r="H17" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="I17" s="15" t="n">
         <v>43381</v>
       </c>
-      <c r="J17" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17" s="12"/>
-      <c r="N17" s="13" t="s">
-        <v>28</v>
+      <c r="J17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="N17" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="O17" s="15" t="n">
         <v>43416</v>
       </c>
-      <c r="P17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="P17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="W17" s="13"/>
+      <c r="X17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13" t="s">
-        <v>8</v>
+      <c r="B18" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>43394</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="14"/>
+      <c r="D18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="16"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="13" t="s">
-        <v>8</v>
+      <c r="H18" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="I18" s="15" t="n">
         <v>43394</v>
       </c>
-      <c r="J18" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" s="14"/>
-      <c r="N18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R18" s="14"/>
+      <c r="J18" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="16"/>
+      <c r="N18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R18" s="16"/>
+      <c r="T18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U18" s="15" t="n">
+        <v>43383</v>
+      </c>
+      <c r="V18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="W18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="X18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="13" t="s">
-        <v>8</v>
+      <c r="B19" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C19" s="15" t="n">
         <v>43394</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="14"/>
+      <c r="D19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="16"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="13" t="s">
-        <v>8</v>
+      <c r="H19" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="I19" s="15" t="n">
         <v>43395</v>
       </c>
-      <c r="J19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" s="14"/>
-      <c r="N19" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R19" s="14"/>
+      <c r="J19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="N19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="16"/>
+      <c r="T19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U19" s="15" t="n">
+        <v>43383</v>
+      </c>
+      <c r="V19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="W19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="X19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="13" t="s">
-        <v>38</v>
+      <c r="B20" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="16"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="13" t="s">
-        <v>8</v>
+      <c r="H20" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="I20" s="15" t="n">
         <v>43395</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="14"/>
-      <c r="N20" s="13" t="s">
+      <c r="J20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="N20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R20" s="16"/>
+      <c r="T20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U20" s="15" t="n">
+        <v>43390</v>
+      </c>
+      <c r="V20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R20" s="14"/>
+      <c r="W20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="X20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="13" t="s">
-        <v>43</v>
+      <c r="B21" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>45</v>
+        <v>29</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="13" t="s">
-        <v>38</v>
+      <c r="H21" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="I21" s="15" t="n">
         <v>43404</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21" s="14"/>
-      <c r="N21" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="R21" s="14" t="s">
-        <v>50</v>
+      <c r="J21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="16"/>
+      <c r="N21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U21" s="15" t="n">
+        <v>43392</v>
+      </c>
+      <c r="V21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="W21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="X21" s="16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="48.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>53</v>
+      <c r="D22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="13" t="s">
-        <v>38</v>
+      <c r="H22" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="I22" s="15" t="n">
         <v>43411</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="16"/>
+      <c r="N22" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22" s="15" t="n">
+        <v>43390</v>
+      </c>
+      <c r="V22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="W22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="X22" s="16"/>
+    </row>
+    <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="14"/>
-      <c r="N22" s="13" t="s">
+      <c r="K23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14" t="s">
+      <c r="N23" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="Q22" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="R22" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="N23" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="O23" s="17" t="n">
         <v>43429</v>
       </c>
-      <c r="P23" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q23" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="R23" s="14" t="s">
-        <v>65</v>
-      </c>
+      <c r="P23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="V23" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="W23" s="13"/>
+      <c r="X23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="59.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="s">
-        <v>43</v>
+      <c r="B24" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>11</v>
+        <v>61</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>69</v>
+      <c r="H24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="O24" s="20" t="n">
         <v>43429</v>
       </c>
       <c r="P24" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q24" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="T24" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="U24" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="V24" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="W24" s="13"/>
+      <c r="X24" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Q24" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="R24" s="18" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="E25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="14" t="s">
+      <c r="G25" s="6"/>
+      <c r="H25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="16"/>
+      <c r="N25" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="14"/>
-      <c r="N25" s="19" t="s">
+      <c r="O25" s="24"/>
+      <c r="P25" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23" t="s">
+      <c r="Q25" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="R25" s="26"/>
+      <c r="T25" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="U25" s="15" t="n">
+        <v>43390</v>
+      </c>
+      <c r="V25" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="25"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>43429</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="14" t="s">
+      <c r="E26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>78</v>
       </c>
       <c r="G26" s="6"/>
-      <c r="H26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J26" s="14" t="s">
+      <c r="H26" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="K26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26" s="14"/>
-      <c r="N26" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14" t="s">
+      <c r="K26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="16"/>
+      <c r="N26" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="14"/>
+      <c r="Q26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R26" s="16"/>
+      <c r="T26" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="U26" s="15" t="n">
+        <v>43383</v>
+      </c>
+      <c r="V26" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="W26" s="13"/>
+      <c r="X26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="37.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>43429</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="14" t="s">
+      <c r="D27" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>78</v>
       </c>
       <c r="G27" s="6"/>
-      <c r="H27" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="14" t="s">
+      <c r="H27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N27" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14" t="s">
+      <c r="K27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="14" t="s">
+      <c r="N27" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16" t="s">
         <v>85</v>
       </c>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="52.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C28" s="15"/>
-      <c r="D28" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="14"/>
+      <c r="D28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="16"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" s="14" t="s">
+      <c r="H28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="N28" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14" t="s">
+      <c r="K28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="14" t="s">
+      <c r="N28" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16" t="s">
         <v>90</v>
       </c>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="16" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>90</v>
-      </c>
       <c r="G29" s="6"/>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="14" t="s">
         <v>76</v>
       </c>
       <c r="I29" s="17" t="n">
         <v>43429</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L29" s="14"/>
-      <c r="N29" s="13" t="s">
+      <c r="J29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14" t="s">
+      <c r="K29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="16"/>
+      <c r="N29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="14" t="s">
-        <v>90</v>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13"/>
+      <c r="B30" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="C30" s="15"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="14"/>
+      <c r="D30" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="6"/>
       <c r="H30" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="J30" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="K30" s="24"/>
-      <c r="L30" s="25" t="s">
-        <v>73</v>
+        <v>34</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="25"/>
+      <c r="L30" s="26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I31" s="26" t="n">
+      <c r="I31" s="27" t="n">
         <v>43430</v>
       </c>
-      <c r="J31" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="L31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="J32" s="13" t="s">
+      <c r="I32" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="14" t="n">
+        <v>43430</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="K35" s="29"/>
+      <c r="L35" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="K36" s="29"/>
+      <c r="L36" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="K37" s="29"/>
+      <c r="L37" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="K38" s="29"/>
+      <c r="L38" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="K39" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="K40" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="L40" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H41" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I41" s="15"/>
+      <c r="J41" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="6"/>
-      <c r="H33" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-    </row>
-    <row r="34" customFormat="false" ht="60.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G34" s="6"/>
-      <c r="H34" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I34" s="13" t="n">
-        <v>43430</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="36.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="27" t="s">
+      <c r="K41" s="13"/>
+      <c r="L41" s="16"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I42" s="15"/>
+      <c r="J42" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="K35" s="28"/>
-      <c r="L35" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="K36" s="28"/>
-      <c r="L36" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27" t="s">
+      <c r="K42" s="13"/>
+      <c r="L42" s="16"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="15"/>
+      <c r="J43" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="K37" s="28"/>
-      <c r="L37" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="K38" s="28"/>
-      <c r="L38" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="K40" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="L40" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="16"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="14"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>

</xml_diff>